<commit_message>
Update AttributeMapping import to use first column as ID by default. Fix tests
</commit_message>
<xml_diff>
--- a/test/data/AM1.xlsx
+++ b/test/data/AM1.xlsx
@@ -17,13 +17,13 @@
     <t>Attribute</t>
   </si>
   <si>
-    <t>Attribute Ontology</t>
+    <t>Attribute Ontology ID</t>
   </si>
   <si>
     <t>Unit</t>
   </si>
   <si>
-    <t>Unit Ontology</t>
+    <t>Unit Ontology ID</t>
   </si>
   <si>
     <t>S1</t>

</xml_diff>